<commit_message>
added many sections + fixed buttons with empty imgs
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel\Desktop\DEV\Projects\habsora-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ABE1CB-3312-4B32-B1BD-BD23CA972EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B92FABD-81BC-42F9-95AF-A058261DEAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{71E22AE3-B8F2-4D0F-8307-C2EF0999BC5A}"/>
+    <workbookView xWindow="4785" yWindow="1410" windowWidth="21600" windowHeight="11295" xr2:uid="{71E22AE3-B8F2-4D0F-8307-C2EF0999BC5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="400">
   <si>
     <t>Yeshúa es ungido en Betania</t>
   </si>
@@ -1146,7 +1146,85 @@
     <t>Parábola del hijo pródigo</t>
   </si>
   <si>
-    <t>15:11</t>
+    <t>15:1-10</t>
+  </si>
+  <si>
+    <t>Parábolas de la oveja y de la moneda perdidas</t>
+  </si>
+  <si>
+    <t>Cuando la sal pierde su sabor</t>
+  </si>
+  <si>
+    <t>14:34-35</t>
+  </si>
+  <si>
+    <t>Lo que cuesta seguir a Yeshúa</t>
+  </si>
+  <si>
+    <t>14:25-33</t>
+  </si>
+  <si>
+    <t>14:15-24</t>
+  </si>
+  <si>
+    <t>Parábola de la gran cena</t>
+  </si>
+  <si>
+    <t>Los convidados a las bodas</t>
+  </si>
+  <si>
+    <t>14:7-14</t>
+  </si>
+  <si>
+    <t>Yeshúa sana a un hidrópico (enseñanza sobre el Shabat)</t>
+  </si>
+  <si>
+    <t>14:1-6</t>
+  </si>
+  <si>
+    <t>13:31-35</t>
+  </si>
+  <si>
+    <t>Lamento sobre Jerusalén tras ser advertido sobre Herodes</t>
+  </si>
+  <si>
+    <t>13:22-30</t>
+  </si>
+  <si>
+    <t>La puerta estrecha</t>
+  </si>
+  <si>
+    <t>13:1</t>
+  </si>
+  <si>
+    <t>Parábola de la levadura</t>
+  </si>
+  <si>
+    <t>Parábola de la semilla de mostaza</t>
+  </si>
+  <si>
+    <t>Yeshúa sana a una mujer en Shabat</t>
+  </si>
+  <si>
+    <t>Parábola de la higuera estéril</t>
+  </si>
+  <si>
+    <t>Arrepentíos o pereceréis</t>
+  </si>
+  <si>
+    <t>13:1-5</t>
+  </si>
+  <si>
+    <t>13:6-9</t>
+  </si>
+  <si>
+    <t>13:10-17</t>
+  </si>
+  <si>
+    <t>13:18-19</t>
+  </si>
+  <si>
+    <t>13:20-21</t>
   </si>
 </sst>
 </file>
@@ -1624,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E032C8F5-6262-462E-BCEC-F76232E36E44}">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,14 +1775,14 @@
         <v>24621</v>
       </c>
       <c r="C4" s="10">
-        <v>15799</v>
+        <v>13584</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" si="0"/>
-        <v>0.35831201007270219</v>
+        <v>0.44827586206896552</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>373</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1735,11 +1813,11 @@
       </c>
       <c r="C6" s="10">
         <f>C5+C4+C3+C2</f>
-        <v>48200</v>
+        <v>45985</v>
       </c>
       <c r="D6" s="17">
         <f>(B6-C6)/B6</f>
-        <v>0.38911561177156473</v>
+        <v>0.41718841094015363</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2159,11 +2237,11 @@
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22" t="s">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -2172,75 +2250,63 @@
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18" t="s">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="F36" s="18"/>
       <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18" t="s">
-        <v>368</v>
+        <v>397</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="F37" s="18"/>
       <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>366</v>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18" t="s">
+        <v>398</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="F38" s="18"/>
       <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18" t="s">
-        <v>358</v>
+        <v>399</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="F39" s="18"/>
       <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="22" t="s">
-        <v>327</v>
+        <v>388</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>363</v>
@@ -2251,11 +2317,11 @@
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="22" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>363</v>
@@ -2266,11 +2332,11 @@
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="22" t="s">
-        <v>354</v>
+        <v>383</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>363</v>
@@ -2281,11 +2347,11 @@
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18" t="s">
-        <v>353</v>
+        <v>382</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="22" t="s">
-        <v>352</v>
+        <v>381</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>363</v>
@@ -2296,11 +2362,11 @@
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18" t="s">
-        <v>350</v>
+        <v>379</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="22" t="s">
-        <v>351</v>
+        <v>380</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>363</v>
@@ -2311,11 +2377,11 @@
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18" t="s">
-        <v>348</v>
+        <v>378</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="22" t="s">
-        <v>349</v>
+        <v>377</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>363</v>
@@ -2326,11 +2392,11 @@
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18" t="s">
-        <v>347</v>
+        <v>376</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="22" t="s">
-        <v>346</v>
+        <v>375</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>363</v>
@@ -2338,322 +2404,307 @@
       <c r="G46" s="18"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G47" s="18"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G49" s="18"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D53" s="21"/>
+      <c r="E53" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G57" s="18"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B60" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C60" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E60" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B61" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C61" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E61" s="20" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B62" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C62" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E62" s="20" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E63" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" t="s">
+      <c r="D64" s="7"/>
+      <c r="E64" t="s">
         <v>241</v>
       </c>
-      <c r="I51" s="8"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="10"/>
-      <c r="C52" s="10" t="s">
+      <c r="I64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="10"/>
+      <c r="C65" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" t="s">
+      <c r="D65" s="7"/>
+      <c r="E65" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B66" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C66" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" t="s">
+      <c r="D66" s="10"/>
+      <c r="E66" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E54" t="s">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E55" t="s">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E56" t="s">
-        <v>2</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" t="s">
-        <v>3</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E58" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D60" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E60" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E62" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E66" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>186</v>
+        <v>213</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>249</v>
@@ -2663,17 +2714,11 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>220</v>
+      <c r="D68" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>249</v>
@@ -2682,15 +2727,21 @@
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>182</v>
+        <v>207</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="E69" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>249</v>
@@ -2700,17 +2751,12 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>221</v>
-      </c>
+      <c r="C70" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70" s="8"/>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>249</v>
@@ -2719,18 +2765,21 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>177</v>
+        <v>202</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="E71" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>249</v>
@@ -2740,91 +2789,65 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>249</v>
-      </c>
+      <c r="D72" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="2"/>
       <c r="G72" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>249</v>
-      </c>
+      <c r="D73" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="2"/>
       <c r="G73" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>249</v>
-      </c>
+      <c r="D74" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="2"/>
       <c r="G74" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>249</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="2"/>
       <c r="G75" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>22</v>
+        <v>195</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>249</v>
@@ -2834,14 +2857,17 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="B77" s="2" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>23</v>
+        <v>191</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>249</v>
@@ -2852,16 +2878,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>24</v>
+        <v>189</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>249</v>
@@ -2872,16 +2895,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>25</v>
+        <v>219</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>249</v>
@@ -2892,16 +2915,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>26</v>
+        <v>186</v>
+      </c>
+      <c r="E80" t="s">
+        <v>13</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>249</v>
@@ -2912,13 +2929,16 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>27</v>
+        <v>184</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>249</v>
@@ -2929,16 +2949,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>28</v>
+        <v>182</v>
+      </c>
+      <c r="E82" t="s">
+        <v>15</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>249</v>
@@ -2949,13 +2966,16 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>29</v>
+        <v>180</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E83" t="s">
+        <v>16</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>249</v>
@@ -2966,16 +2986,16 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>30</v>
+        <v>177</v>
+      </c>
+      <c r="E84" t="s">
+        <v>17</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>249</v>
@@ -2986,16 +3006,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>249</v>
@@ -3006,16 +3023,16 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>142</v>
+        <v>174</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>249</v>
@@ -3026,13 +3043,16 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>140</v>
+        <v>172</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>249</v>
@@ -3043,10 +3063,16 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>138</v>
+        <v>171</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>249</v>
@@ -3057,10 +3083,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>137</v>
+        <v>168</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>249</v>
@@ -3070,11 +3099,14 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>136</v>
+      <c r="B90" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>249</v>
@@ -3085,19 +3117,16 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>249</v>
@@ -3107,17 +3136,17 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>131</v>
+      <c r="A92" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>249</v>
@@ -3128,16 +3157,16 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>226</v>
+        <v>157</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>249</v>
@@ -3146,21 +3175,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>216</v>
+        <v>155</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>249</v>
@@ -3170,20 +3193,17 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>121</v>
+      <c r="A95" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>249</v>
@@ -3194,19 +3214,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>249</v>
@@ -3217,19 +3231,16 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>249</v>
@@ -3239,20 +3250,17 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>112</v>
+      <c r="A98" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>249</v>
@@ -3262,11 +3270,17 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D99" s="2" t="s">
-        <v>110</v>
+      <c r="A99" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>249</v>
@@ -3275,18 +3289,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>249</v>
@@ -3297,19 +3308,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>249</v>
@@ -3320,19 +3322,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>249</v>
@@ -3343,19 +3336,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>249</v>
@@ -3365,11 +3349,20 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="C104" s="2" t="s">
-        <v>95</v>
+        <v>133</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>249</v>
@@ -3379,17 +3372,17 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>94</v>
+      <c r="A105" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>249</v>
@@ -3400,16 +3393,16 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>89</v>
+        <v>128</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>249</v>
@@ -3418,12 +3411,21 @@
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="D107" s="2" t="s">
-        <v>88</v>
+        <v>216</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>249</v>
@@ -3433,20 +3435,20 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D108" s="4">
-        <v>0.80347222222222225</v>
+      <c r="A108" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>249</v>
@@ -3457,19 +3459,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>249</v>
@@ -3480,19 +3482,19 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>229</v>
+        <v>115</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>249</v>
@@ -3502,11 +3504,20 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>80</v>
+      <c r="A111" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>249</v>
@@ -3516,18 +3527,31 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E112" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>79</v>
+        <v>109</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>249</v>
@@ -3537,17 +3561,20 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B114" s="2" t="s">
-        <v>78</v>
+        <v>218</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>249</v>
@@ -3557,17 +3584,20 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>75</v>
+      <c r="A115" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>249</v>
@@ -3577,11 +3607,20 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D116" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>249</v>
@@ -3591,14 +3630,11 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>71</v>
+      <c r="C117" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>249</v>
@@ -3608,11 +3644,17 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D118" s="2" t="s">
-        <v>70</v>
+      <c r="A118" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>249</v>
@@ -3623,33 +3665,256 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D121" s="4">
+        <v>0.80347222222222225</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E125" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D129" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F119" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D120" t="s">
+      <c r="F132" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
         <v>66</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E133" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2" t="s">
+      <c r="F133" s="2"/>
+      <c r="G133" s="2" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
we got to Capernaum!
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel\Desktop\DEV\Projects\habsora-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B92FABD-81BC-42F9-95AF-A058261DEAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131D8919-EDF4-4067-A0D0-B9933CA8DC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1410" windowWidth="21600" windowHeight="11295" xr2:uid="{71E22AE3-B8F2-4D0F-8307-C2EF0999BC5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71E22AE3-B8F2-4D0F-8307-C2EF0999BC5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="447">
   <si>
     <t>Yeshúa es ungido en Betania</t>
   </si>
@@ -1194,9 +1194,6 @@
     <t>La puerta estrecha</t>
   </si>
   <si>
-    <t>13:1</t>
-  </si>
-  <si>
     <t>Parábola de la levadura</t>
   </si>
   <si>
@@ -1225,6 +1222,150 @@
   </si>
   <si>
     <t>13:20-21</t>
+  </si>
+  <si>
+    <t>12:57-59</t>
+  </si>
+  <si>
+    <t>Arréglate con tu adversario</t>
+  </si>
+  <si>
+    <t>12:54-56</t>
+  </si>
+  <si>
+    <t>¿Cómo no reconocéis este tiempo?</t>
+  </si>
+  <si>
+    <t>12:49-53</t>
+  </si>
+  <si>
+    <t>Yeshúa, causa de división</t>
+  </si>
+  <si>
+    <t>El siervo vigilante y el siervo infiel</t>
+  </si>
+  <si>
+    <t>12:35-48</t>
+  </si>
+  <si>
+    <t>12:32-34</t>
+  </si>
+  <si>
+    <t>Tesoros en los cielos</t>
+  </si>
+  <si>
+    <t>12:22-31</t>
+  </si>
+  <si>
+    <t>El afán y la ansiedad</t>
+  </si>
+  <si>
+    <t>12:13-21</t>
+  </si>
+  <si>
+    <t>El rico insensato</t>
+  </si>
+  <si>
+    <t>12:8-12</t>
+  </si>
+  <si>
+    <t>12:4-7</t>
+  </si>
+  <si>
+    <t>A quién se debe temer</t>
+  </si>
+  <si>
+    <t>12:1-3</t>
+  </si>
+  <si>
+    <t>11:37-54</t>
+  </si>
+  <si>
+    <t>Yeshúa acusa a fariseos y a intérpretes de la Torah</t>
+  </si>
+  <si>
+    <t>11:33-36</t>
+  </si>
+  <si>
+    <t>La lámapara del cuerpo</t>
+  </si>
+  <si>
+    <t>11:29-32</t>
+  </si>
+  <si>
+    <t>La generación perversa demanda señal</t>
+  </si>
+  <si>
+    <t>11:27-28</t>
+  </si>
+  <si>
+    <t>Los que en verdad son bienaventurados</t>
+  </si>
+  <si>
+    <t>11:24-26</t>
+  </si>
+  <si>
+    <t>El espíritu inmundo que vuelve</t>
+  </si>
+  <si>
+    <t>11:14-21</t>
+  </si>
+  <si>
+    <t>Una casa dividida contra sí misma</t>
+  </si>
+  <si>
+    <t>11:1-13</t>
+  </si>
+  <si>
+    <t>Yeshúa y la oración</t>
+  </si>
+  <si>
+    <t>Parábola del buen samaritano</t>
+  </si>
+  <si>
+    <t>10:25-37</t>
+  </si>
+  <si>
+    <t>10:38-42</t>
+  </si>
+  <si>
+    <t>Yeshúa visita a Marta y a María</t>
+  </si>
+  <si>
+    <t>10:21-24</t>
+  </si>
+  <si>
+    <t>Yeshúa se regocija</t>
+  </si>
+  <si>
+    <t>10:17-20</t>
+  </si>
+  <si>
+    <t>Regreso de los 70</t>
+  </si>
+  <si>
+    <t>10:13-16</t>
+  </si>
+  <si>
+    <t>Ayes sobre las ciudades que no se arrepintieron</t>
+  </si>
+  <si>
+    <t>10:1-12</t>
+  </si>
+  <si>
+    <t>Misión de los 70</t>
+  </si>
+  <si>
+    <t>9:57-62</t>
+  </si>
+  <si>
+    <t>Los que querían seguir a Yeshúa</t>
+  </si>
+  <si>
+    <t>9:57</t>
+  </si>
+  <si>
+    <t>Confesar a Yeshúa y la blasfemia contra el Espíritu Santo</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E032C8F5-6262-462E-BCEC-F76232E36E44}">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,17 +1913,17 @@
         <v>236</v>
       </c>
       <c r="B4" s="10">
-        <v>24621</v>
+        <v>24862</v>
       </c>
       <c r="C4" s="10">
-        <v>13584</v>
+        <v>10266</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" si="0"/>
-        <v>0.44827586206896552</v>
+        <v>0.58708068538331593</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>389</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1809,15 +1950,15 @@
       </c>
       <c r="B6" s="10">
         <f>B5+B4+B3+B2</f>
-        <v>78902</v>
+        <v>79143</v>
       </c>
       <c r="C6" s="10">
         <f>C5+C4+C3+C2</f>
-        <v>45985</v>
+        <v>42667</v>
       </c>
       <c r="D6" s="17">
         <f>(B6-C6)/B6</f>
-        <v>0.41718841094015363</v>
+        <v>0.46088725471614672</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2236,26 +2377,18 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="18" t="s">
-        <v>395</v>
-      </c>
+      <c r="C35" s="18"/>
       <c r="D35" s="21"/>
-      <c r="E35" s="22" t="s">
-        <v>394</v>
-      </c>
+      <c r="E35" s="22"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
-      <c r="C36" s="18" t="s">
-        <v>396</v>
-      </c>
+      <c r="C36" s="18"/>
       <c r="D36" s="21"/>
-      <c r="E36" s="22" t="s">
-        <v>393</v>
-      </c>
+      <c r="E36" s="22"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
     </row>
@@ -2263,11 +2396,11 @@
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18" t="s">
-        <v>397</v>
+        <v>443</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22" t="s">
-        <v>392</v>
+        <v>444</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
@@ -2276,11 +2409,11 @@
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18" t="s">
-        <v>398</v>
+        <v>441</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22" t="s">
-        <v>391</v>
+        <v>442</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -2289,11 +2422,11 @@
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18" t="s">
-        <v>399</v>
+        <v>439</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="22" t="s">
-        <v>390</v>
+        <v>440</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
@@ -2302,1030 +2435,890 @@
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18" t="s">
-        <v>387</v>
+        <v>437</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="22" t="s">
-        <v>388</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="F40" s="18"/>
       <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18" t="s">
-        <v>385</v>
+        <v>435</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="22" t="s">
-        <v>386</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="F41" s="18"/>
       <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18" t="s">
-        <v>384</v>
+        <v>432</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="22" t="s">
-        <v>383</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="F42" s="18"/>
       <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18" t="s">
-        <v>382</v>
+        <v>433</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="22" t="s">
-        <v>381</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="F43" s="18"/>
       <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18" t="s">
-        <v>379</v>
+        <v>429</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="F44" s="18"/>
       <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18" t="s">
-        <v>378</v>
+        <v>427</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="F45" s="18"/>
       <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18" t="s">
-        <v>376</v>
+        <v>425</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="22" t="s">
-        <v>375</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="F46" s="18"/>
       <c r="G46" s="18"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18" t="s">
-        <v>373</v>
+        <v>423</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="22" t="s">
-        <v>374</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="F47" s="18"/>
       <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
-      <c r="C48" s="18" t="s">
-        <v>371</v>
+      <c r="C48" s="23" t="s">
+        <v>421</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="F48" s="18"/>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18" t="s">
-        <v>370</v>
+        <v>419</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="F49" s="18"/>
       <c r="G49" s="18"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18" t="s">
-        <v>368</v>
+        <v>417</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="F50" s="18"/>
       <c r="G50" s="18"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>366</v>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18" t="s">
+        <v>416</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="F51" s="18"/>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18" t="s">
-        <v>358</v>
+        <v>414</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="F52" s="18"/>
       <c r="G52" s="18"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="18"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18" t="s">
-        <v>331</v>
+        <v>413</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="F53" s="18"/>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18" t="s">
-        <v>356</v>
+        <v>411</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="F54" s="18"/>
       <c r="G54" s="18"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18" t="s">
-        <v>355</v>
+        <v>409</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="F55" s="18"/>
       <c r="G55" s="18"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18" t="s">
-        <v>353</v>
+        <v>407</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="F56" s="18"/>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="18" t="s">
-        <v>350</v>
+        <v>406</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="F57" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="F57" s="18"/>
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="18" t="s">
-        <v>348</v>
+        <v>403</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>363</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="F58" s="18"/>
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18" t="s">
-        <v>347</v>
+        <v>401</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G66" s="18"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G67" s="18"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G68" s="18"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="D69" s="21"/>
+      <c r="E69" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="F69" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G69" s="18"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="D70" s="21"/>
+      <c r="E70" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G70" s="18"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="F71" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G71" s="18"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="18"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="D72" s="21"/>
+      <c r="E72" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="F72" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G72" s="18"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="18"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="D73" s="21"/>
+      <c r="E73" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G73" s="18"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D74" s="21"/>
+      <c r="E74" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G74" s="18"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="D75" s="21"/>
+      <c r="E75" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G75" s="18"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="D76" s="21"/>
+      <c r="E76" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="D77" s="21"/>
+      <c r="E77" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D78" s="21"/>
+      <c r="E78" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G78" s="18"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D79" s="21"/>
+      <c r="E79" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G79" s="18"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="21"/>
+      <c r="E80" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="F80" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D81" s="21"/>
+      <c r="E81" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="F81" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G81" s="18"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D82" s="21"/>
+      <c r="E82" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="F82" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G82" s="18"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D83" s="21"/>
+      <c r="E83" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G83" s="18"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="18"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D84" s="21"/>
+      <c r="E84" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="F84" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G84" s="18"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="18"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D85" s="21"/>
+      <c r="E85" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F85" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="G59" s="18"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="G85" s="18"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B86" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="C86" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E86" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B87" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C87" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E87" s="20" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B88" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C88" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E88" s="20" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B89" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E89" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="10" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C90" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D64" s="7"/>
-      <c r="E64" t="s">
+      <c r="D90" s="7"/>
+      <c r="E90" t="s">
         <v>241</v>
       </c>
-      <c r="I64" s="8"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="10"/>
-      <c r="C65" s="10" t="s">
+      <c r="I90" s="8"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="10"/>
+      <c r="C91" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" t="s">
+      <c r="D91" s="7"/>
+      <c r="E91" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B92" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C92" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" t="s">
+      <c r="D92" s="10"/>
+      <c r="E92" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E93" t="s">
         <v>0</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+      <c r="F93" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E94" t="s">
         <v>1</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="F94" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E95" t="s">
         <v>2</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="6" t="s">
+      <c r="F95" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C96" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D70" s="8"/>
-      <c r="E70" t="s">
+      <c r="D96" s="8"/>
+      <c r="E96" t="s">
         <v>3</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="F96" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E97" t="s">
         <v>4</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+      <c r="F97" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E98" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="2" t="s">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E99" t="s">
         <v>6</v>
       </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D74" s="2" t="s">
+      <c r="F99" s="2"/>
+      <c r="G99" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E100" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" t="s">
-        <v>8</v>
-      </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E76" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E77" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E78" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E79" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E81" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E82" t="s">
-        <v>15</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E83" t="s">
-        <v>16</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E84" t="s">
-        <v>17</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>249</v>
-      </c>
+      <c r="F100" s="2"/>
       <c r="G100" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>249</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E101" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="2"/>
       <c r="G101" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>35</v>
+        <v>195</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E102" t="s">
+        <v>9</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>249</v>
@@ -3336,10 +3329,16 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>36</v>
+        <v>193</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>249</v>
@@ -3350,19 +3349,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>37</v>
+        <v>189</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>249</v>
@@ -3372,17 +3365,17 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>131</v>
+      <c r="A105" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>38</v>
+        <v>219</v>
+      </c>
+      <c r="E105" t="s">
+        <v>12</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>249</v>
@@ -3393,16 +3386,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>39</v>
+        <v>186</v>
+      </c>
+      <c r="E106" t="s">
+        <v>13</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>249</v>
@@ -3411,21 +3398,18 @@
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>126</v>
+        <v>184</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>40</v>
+        <v>220</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>249</v>
@@ -3435,20 +3419,14 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>41</v>
+      <c r="A108" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>249</v>
@@ -3459,19 +3437,16 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>42</v>
+        <v>221</v>
+      </c>
+      <c r="E109" t="s">
+        <v>16</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>249</v>
@@ -3482,19 +3457,16 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>43</v>
+        <v>177</v>
+      </c>
+      <c r="E110" t="s">
+        <v>17</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>249</v>
@@ -3504,20 +3476,14 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>217</v>
+      <c r="A111" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>249</v>
@@ -3527,11 +3493,17 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D112" s="2" t="s">
-        <v>110</v>
+      <c r="A112" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>249</v>
@@ -3540,18 +3512,18 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>249</v>
@@ -3562,19 +3534,16 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>104</v>
+        <v>171</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>249</v>
@@ -3585,19 +3554,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>100</v>
+        <v>168</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>249</v>
@@ -3607,20 +3570,14 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="B116" s="2" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>249</v>
@@ -3630,11 +3587,17 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="C117" s="2" t="s">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>249</v>
@@ -3645,16 +3608,16 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>249</v>
@@ -3665,16 +3628,16 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>89</v>
+        <v>158</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>249</v>
@@ -3684,11 +3647,14 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D120" s="2" t="s">
-        <v>88</v>
+      <c r="A120" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>249</v>
@@ -3698,20 +3664,17 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>215</v>
+      <c r="A121" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D121" s="4">
-        <v>0.80347222222222225</v>
+        <v>152</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>249</v>
@@ -3722,19 +3685,13 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>249</v>
@@ -3745,19 +3702,16 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>249</v>
@@ -3768,10 +3722,16 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>80</v>
+        <v>146</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>249</v>
@@ -3781,18 +3741,34 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="E125" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>79</v>
+        <v>139</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>249</v>
@@ -3802,17 +3778,11 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>76</v>
+      <c r="A127" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>249</v>
@@ -3822,17 +3792,11 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B128" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>74</v>
+      <c r="A128" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>249</v>
@@ -3842,11 +3806,11 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D129" s="2" t="s">
-        <v>73</v>
+      <c r="A129" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>249</v>
@@ -3857,13 +3821,19 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>71</v>
+        <v>134</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>249</v>
@@ -3873,11 +3843,17 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D131" s="2" t="s">
-        <v>70</v>
+      <c r="A131" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>249</v>
@@ -3888,33 +3864,528 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D138" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C143" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D146" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D147" s="4">
+        <v>0.80347222222222225</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E151" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B153" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D155" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D157" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G157" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F132" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D133" t="s">
+      <c r="F158" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G158" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
         <v>66</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2" t="s">
+      <c r="F159" s="2"/>
+      <c r="G159" s="2" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>